<commit_message>
question 1 Vandy players salaries
</commit_message>
<xml_diff>
--- a/Lahman Answers.xlsx
+++ b/Lahman Answers.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\vmware-host\Shared Folders\Documents\NSS_Data_Analytics\Projects\lahaman-baseball-maureencaballero\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{6712DFD0-423D-4001-BBF6-AF1FC2993870}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{15E2D91B-7133-42E7-A01D-31799530B533}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="300" windowWidth="14235" windowHeight="12008" xr2:uid="{E022E7C2-3455-400F-AFE4-B3C83D196596}"/>
   </bookViews>
@@ -83,7 +83,7 @@
     <t>It is thought that since left-handed pitchers are more rare, causing batters to face them less often, that they are more effective. Investigate this claim and present evidence to either support or dispute this claim. First, determine just how rare left-handed pitchers are compared with right-handed pitchers. Are left-handed pitchers more likely to win the Cy Young Award? Are they more likely to make it into the hall of fame?</t>
   </si>
   <si>
-    <t>wer</t>
+    <t>1871-2016</t>
   </si>
 </sst>
 </file>
@@ -438,7 +438,7 @@
   <dimension ref="A1:A29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -530,5 +530,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>